<commit_message>
Alpha version of root rot extension.
</commit_message>
<xml_diff>
--- a/Docs/Root Rot equations.xlsx
+++ b/Docs/Root Rot equations.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>ph</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>p(S:I)</t>
   </si>
@@ -83,6 +80,15 @@
   <si>
     <t>maxProbDI</t>
   </si>
+  <si>
+    <t>Calculated Values</t>
+  </si>
+  <si>
+    <t>User Inputs</t>
+  </si>
+  <si>
+    <t>pressure head (mm)</t>
+  </si>
 </sst>
 </file>
 
@@ -97,7 +103,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,8 +116,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,13 +137,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -183,6 +217,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -447,11 +482,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="252379000"/>
-        <c:axId val="252376256"/>
+        <c:axId val="433830032"/>
+        <c:axId val="433832384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="252379000"/>
+        <c:axId val="433830032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -499,6 +534,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -565,12 +601,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252376256"/>
+        <c:crossAx val="433832384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252376256"/>
+        <c:axId val="433832384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -617,6 +653,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -683,7 +720,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252379000"/>
+        <c:crossAx val="433830032"/>
         <c:crossesAt val="-25"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1084,11 +1121,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="252373120"/>
-        <c:axId val="252371552"/>
+        <c:axId val="433834736"/>
+        <c:axId val="433832776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="252373120"/>
+        <c:axId val="433834736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1202,12 +1239,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252371552"/>
+        <c:crossAx val="433832776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252371552"/>
+        <c:axId val="433832776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1321,7 +1358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252373120"/>
+        <c:crossAx val="433834736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1367,6 +1404,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1781,11 +1819,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="252372728"/>
-        <c:axId val="252371944"/>
+        <c:axId val="433829640"/>
+        <c:axId val="433833560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="252372728"/>
+        <c:axId val="433829640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -1899,12 +1937,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252371944"/>
+        <c:crossAx val="433833560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252371944"/>
+        <c:axId val="433833560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2018,7 +2056,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252372728"/>
+        <c:crossAx val="433829640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2419,11 +2457,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="252376648"/>
-        <c:axId val="252372336"/>
+        <c:axId val="433835520"/>
+        <c:axId val="433830424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="252376648"/>
+        <c:axId val="433835520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -2537,12 +2575,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252372336"/>
+        <c:crossAx val="433830424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252372336"/>
+        <c:axId val="433830424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2656,7 +2694,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252376648"/>
+        <c:crossAx val="433835520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4935,15 +4973,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>271462</xdr:colOff>
+      <xdr:colOff>404812</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>576262</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:colOff>557212</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4973,7 +5011,7 @@
       <cdr:y>0.87326</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.30937</cdr:x>
+      <cdr:x>0.24479</cdr:x>
       <cdr:y>0.9566</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -4983,8 +5021,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="280987" y="2395537"/>
-          <a:ext cx="1133475" cy="228601"/>
+          <a:off x="280995" y="2395527"/>
+          <a:ext cx="838193" cy="228618"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5001,7 +5039,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>LethalTemp = -24</a:t>
+            <a:t>LethalTemp</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5077,15 +5115,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5113,12 +5151,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.14375</cdr:x>
-      <cdr:y>0.85069</cdr:y>
+      <cdr:x>0.19063</cdr:x>
+      <cdr:y>0.80903</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.34375</cdr:x>
-      <cdr:y>0.94097</cdr:y>
+      <cdr:x>0.31146</cdr:x>
+      <cdr:y>0.89931</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -5127,8 +5165,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="657225" y="2333625"/>
-          <a:ext cx="914400" cy="247650"/>
+          <a:off x="871538" y="2219325"/>
+          <a:ext cx="552450" cy="247650"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5145,7 +5183,52 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>phWet = 30</a:t>
+            <a:t>phWet</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.14375</cdr:x>
+      <cdr:y>0.85069</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.275</cdr:x>
+      <cdr:y>0.94097</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="657225" y="2333613"/>
+          <a:ext cx="600075" cy="247656"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>phWet </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5153,11 +5236,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.52986</cdr:x>
+      <cdr:x>0.55278</cdr:x>
       <cdr:y>0.82639</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.72986</cdr:x>
+      <cdr:x>0.66875</cdr:x>
       <cdr:y>0.91667</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -5167,8 +5250,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2422525" y="2266950"/>
-          <a:ext cx="914400" cy="247650"/>
+          <a:off x="2527295" y="2266953"/>
+          <a:ext cx="530230" cy="247656"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5249,7 +5332,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>phDry = 150</a:t>
+            <a:t>phDry </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5257,12 +5340,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.79653</cdr:x>
-      <cdr:y>0.86574</cdr:y>
+      <cdr:x>0.87153</cdr:x>
+      <cdr:y>0.07407</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.99653</cdr:x>
-      <cdr:y>0.95602</cdr:y>
+      <cdr:x>0.98542</cdr:x>
+      <cdr:y>0.16435</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -5271,8 +5354,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3641725" y="2374900"/>
-          <a:ext cx="914400" cy="247650"/>
+          <a:off x="3984636" y="203198"/>
+          <a:ext cx="520690" cy="247656"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5353,7 +5436,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>phMax = 250</a:t>
+            <a:t>phMax</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5365,7 +5448,7 @@
       <cdr:y>0.66435</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.88958</cdr:x>
+      <cdr:x>0.82917</cdr:x>
       <cdr:y>0.75463</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -5375,8 +5458,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2984499" y="1822450"/>
-          <a:ext cx="1082675" cy="247656"/>
+          <a:off x="2984510" y="1822445"/>
+          <a:ext cx="806440" cy="247656"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5457,7 +5540,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>minProbID = 0.1</a:t>
+            <a:t>minProbID</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5466,7 +5549,7 @@
 </c:userShapes>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -5474,7 +5557,7 @@
       <cdr:y>0.20602</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.8125</cdr:x>
+      <cdr:x>0.74375</cdr:x>
       <cdr:y>0.2963</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -5484,8 +5567,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2565400" y="565150"/>
-          <a:ext cx="1149350" cy="247656"/>
+          <a:off x="2565396" y="565154"/>
+          <a:ext cx="835030" cy="247656"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5566,7 +5649,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>maxProbDI = 0.85</a:t>
+            <a:t>maxProbDI</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5574,12 +5657,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.14653</cdr:x>
-      <cdr:y>0.86227</cdr:y>
+      <cdr:x>0.19028</cdr:x>
+      <cdr:y>0.81366</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.34653</cdr:x>
-      <cdr:y>0.95255</cdr:y>
+      <cdr:x>0.31458</cdr:x>
+      <cdr:y>0.90394</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -5588,8 +5671,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="669925" y="2365375"/>
-          <a:ext cx="914400" cy="247656"/>
+          <a:off x="869960" y="2232029"/>
+          <a:ext cx="568315" cy="247656"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5670,7 +5753,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>phWet = 30</a:t>
+            <a:t>phWet</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5678,11 +5761,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.65694</cdr:x>
+      <cdr:x>0.69236</cdr:x>
       <cdr:y>0.86227</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.85694</cdr:x>
+      <cdr:x>0.80833</cdr:x>
       <cdr:y>0.95255</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -5692,8 +5775,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3003550" y="2365375"/>
-          <a:ext cx="914400" cy="247656"/>
+          <a:off x="3165455" y="2365379"/>
+          <a:ext cx="530245" cy="247656"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5774,7 +5857,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>phDry = 150</a:t>
+            <a:t>phDry</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -6046,25 +6129,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>-24</v>
       </c>
     </row>
@@ -6348,6 +6440,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6355,40 +6450,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3"/>
+    </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2">
+      <c r="I2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2">
         <f>(G2+G3)/2</f>
         <v>90</v>
       </c>
@@ -6410,15 +6516,15 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1">
         <v>150</v>
       </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3">
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="2">
         <f>1/(J2-G2)</f>
         <v>1.6666666666666666E-2</v>
       </c>
@@ -6440,15 +6546,15 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1">
         <v>250</v>
       </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4">
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2">
         <f>-1*G2*J3</f>
         <v>-0.5</v>
       </c>
@@ -6470,15 +6576,15 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1">
         <v>0.1</v>
       </c>
-      <c r="I5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5">
+      <c r="I5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="2">
         <f>1/(J2-G3)</f>
         <v>-1.6666666666666666E-2</v>
       </c>
@@ -6500,15 +6606,15 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1">
         <v>0.85</v>
       </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6">
+      <c r="I6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="2">
         <f>-1*G3*(1/(J2-G3))</f>
         <v>2.5</v>
       </c>
@@ -6529,10 +6635,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7">
+      <c r="I7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2">
         <f>(1-G5)/(G4-G3)</f>
         <v>9.0000000000000011E-3</v>
       </c>
@@ -6553,10 +6659,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8">
+      <c r="I8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
         <f>G5-(G3*J7)</f>
         <v>-1.25</v>
       </c>
@@ -7330,6 +7436,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new optional map outputs. User Guide needs updating to reflect these.
</commit_message>
<xml_diff>
--- a/Docs/Root Rot equations.xlsx
+++ b/Docs/Root Rot equations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16935" windowHeight="11970" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16935" windowHeight="11970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dTemp" sheetId="2" r:id="rId1"/>
@@ -481,11 +481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="420513624"/>
-        <c:axId val="420512840"/>
+        <c:axId val="389425856"/>
+        <c:axId val="389426248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="420513624"/>
+        <c:axId val="389425856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -599,12 +599,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420512840"/>
+        <c:crossAx val="389426248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="420512840"/>
+        <c:axId val="389426248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -717,7 +717,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420513624"/>
+        <c:crossAx val="389425856"/>
         <c:crossesAt val="-25"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1425,11 +1425,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="420514800"/>
-        <c:axId val="420518328"/>
+        <c:axId val="326581672"/>
+        <c:axId val="326582848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="420514800"/>
+        <c:axId val="326581672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1544,12 +1544,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420518328"/>
+        <c:crossAx val="326582848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="420518328"/>
+        <c:axId val="326582848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1607,7 +1607,7 @@
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>p(S→I)</a:t>
+                  <a:t>Wetness Index (WI)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1000">
                   <a:effectLst/>
@@ -1696,7 +1696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420514800"/>
+        <c:crossAx val="326581672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2409,11 +2409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="420518720"/>
-        <c:axId val="420511272"/>
+        <c:axId val="328031336"/>
+        <c:axId val="328033688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="420518720"/>
+        <c:axId val="328031336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -2527,12 +2527,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420511272"/>
+        <c:crossAx val="328033688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="420511272"/>
+        <c:axId val="328033688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2657,7 +2657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420518720"/>
+        <c:crossAx val="328031336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3305,11 +3305,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="422245744"/>
-        <c:axId val="422244568"/>
+        <c:axId val="328034080"/>
+        <c:axId val="328029376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="422245744"/>
+        <c:axId val="328034080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -3423,12 +3423,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422244568"/>
+        <c:crossAx val="328029376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="422244568"/>
+        <c:axId val="328029376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3553,7 +3553,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422245744"/>
+        <c:crossAx val="328034080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6159,12 +6159,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.14375</cdr:x>
-      <cdr:y>0.85069</cdr:y>
+      <cdr:x>0.15625</cdr:x>
+      <cdr:y>0.35069</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.275</cdr:x>
-      <cdr:y>0.94097</cdr:y>
+      <cdr:x>0.34375</cdr:x>
+      <cdr:y>0.44097</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -6173,12 +6173,15 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="657225" y="2333613"/>
-          <a:ext cx="600075" cy="247656"/>
+          <a:off x="714375" y="962013"/>
+          <a:ext cx="857250" cy="247656"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -6191,7 +6194,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>phWet </a:t>
+            <a:t>phWet = 51</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -6199,12 +6202,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.55278</cdr:x>
-      <cdr:y>0.82639</cdr:y>
+      <cdr:x>0.25278</cdr:x>
+      <cdr:y>0.68056</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.66875</cdr:x>
-      <cdr:y>0.91667</cdr:y>
+      <cdr:x>0.42708</cdr:x>
+      <cdr:y>0.77084</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -6213,8 +6216,334 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2527295" y="2266953"/>
-          <a:ext cx="530230" cy="247656"/>
+          <a:off x="1155710" y="1866903"/>
+          <a:ext cx="796915" cy="247656"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>phDry = 102 </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.7882</cdr:x>
+      <cdr:y>0.0706</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.99375</cdr:x>
+      <cdr:y>0.16088</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3603635" y="193664"/>
+          <a:ext cx="939790" cy="247656"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>phMax = 250</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.56111</cdr:x>
+      <cdr:y>0.68171</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.80208</cdr:x>
+      <cdr:y>0.77199</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2565410" y="1870070"/>
+          <a:ext cx="1101715" cy="247656"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>minProbID = 0.1</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.48194</cdr:x>
+      <cdr:y>0.20255</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.74583</cdr:x>
+      <cdr:y>0.29283</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2203444" y="555629"/>
+          <a:ext cx="1206505" cy="247656"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -6295,7 +6624,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>phDry </a:t>
+            <a:t>maxProbDI = 0.85</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -6303,12 +6632,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.87153</cdr:x>
-      <cdr:y>0.07407</cdr:y>
+      <cdr:x>0.22361</cdr:x>
+      <cdr:y>0.86227</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.98542</cdr:x>
-      <cdr:y>0.16435</cdr:y>
+      <cdr:x>0.40208</cdr:x>
+      <cdr:y>0.95255</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -6317,8 +6646,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3984636" y="203198"/>
-          <a:ext cx="520690" cy="247656"/>
+          <a:off x="1022359" y="2365382"/>
+          <a:ext cx="815965" cy="247656"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -6399,7 +6728,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>phMax</a:t>
+            <a:t>phWet = 51</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -6407,12 +6736,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.65278</cdr:x>
-      <cdr:y>0.66435</cdr:y>
+      <cdr:x>0.55486</cdr:x>
+      <cdr:y>0.6713</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.82917</cdr:x>
-      <cdr:y>0.75463</cdr:y>
+      <cdr:x>0.73542</cdr:x>
+      <cdr:y>0.76158</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -6421,8 +6750,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2984510" y="1822445"/>
-          <a:ext cx="806440" cy="247656"/>
+          <a:off x="2536820" y="1841504"/>
+          <a:ext cx="825505" cy="247656"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -6503,324 +6832,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>minProbID</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.56111</cdr:x>
-      <cdr:y>0.20602</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.74375</cdr:x>
-      <cdr:y>0.2963</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2565396" y="565154"/>
-          <a:ext cx="835030" cy="247656"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-        </a:ln>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>maxProbDI</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.19028</cdr:x>
-      <cdr:y>0.81366</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.31458</cdr:x>
-      <cdr:y>0.90394</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="4" name="TextBox 1"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="869960" y="2232029"/>
-          <a:ext cx="568315" cy="247656"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-        </a:ln>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>phWet</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.69236</cdr:x>
-      <cdr:y>0.86227</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.80833</cdr:x>
-      <cdr:y>0.95255</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="5" name="TextBox 1"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3165455" y="2365379"/>
-          <a:ext cx="530245" cy="247656"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-        </a:ln>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>phDry</a:t>
+            <a:t>phDry = 102</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -7415,8 +7427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>